<commit_message>
微调 Signed-off-by: tonyshow <994262676@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelToTxtTool/in/卡牌.xlsx
+++ b/ExcelToTxtTool/in/卡牌.xlsx
@@ -290,10 +290,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -301,14 +301,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -326,18 +318,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -348,54 +333,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -410,7 +356,15 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -425,8 +379,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -440,6 +403,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -447,6 +440,13 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -457,49 +457,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,133 +625,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,17 +651,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,7 +678,42 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -705,26 +734,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -739,15 +748,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -756,145 +756,145 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1248,8 +1248,8 @@
   <sheetPr/>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A57"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55:B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -2523,7 +2523,7 @@
         <v>53</v>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="C56">
         <v>5</v>
@@ -2546,7 +2546,7 @@
         <v>54</v>
       </c>
       <c r="B57">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C57">
         <v>5</v>

</xml_diff>